<commit_message>
CHANGE Miilon - Add more vocabulary. Fix a sheet name.
</commit_message>
<xml_diff>
--- a/MiilonData/05_EditoB2_unite4_p59_Le_lieu.xlsx
+++ b/MiilonData/05_EditoB2_unite4_p59_Le_lieu.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GÉNÉRALITÉS" sheetId="1" r:id="rId1"/>
     <sheet name="POUR QUALIFIER UN LIEU" sheetId="2" r:id="rId2"/>
     <sheet name="LOCALISATION" sheetId="3" r:id="rId3"/>
     <sheet name="PAR RAPPORT À UN POINT" sheetId="4" r:id="rId4"/>
+    <sheet name="DISTANCE ET PROXIMITÉ" sheetId="5" r:id="rId5"/>
+    <sheet name="DIRECTION ET MOUVEMENT" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="355">
   <si>
     <t>Mot français</t>
   </si>
@@ -864,6 +866,234 @@
   </si>
   <si>
     <t>v čele, na počátku, v záhlaví čeho</t>
+  </si>
+  <si>
+    <t>aux alentours</t>
+  </si>
+  <si>
+    <t>o.zala~tu:r</t>
+  </si>
+  <si>
+    <t>v okolí</t>
+  </si>
+  <si>
+    <t>contre</t>
+  </si>
+  <si>
+    <t>ko~:tr</t>
+  </si>
+  <si>
+    <t>proti, naproti</t>
+  </si>
+  <si>
+    <t>tout contre</t>
+  </si>
+  <si>
+    <t>tu ko~:tr</t>
+  </si>
+  <si>
+    <t>zcela blízko</t>
+  </si>
+  <si>
+    <t>à côté (de)</t>
+  </si>
+  <si>
+    <t>a ko.te. d@</t>
+  </si>
+  <si>
+    <t>vedle (čeho), mimo</t>
+  </si>
+  <si>
+    <t>au côté de</t>
+  </si>
+  <si>
+    <t>o. ko.te. d@</t>
+  </si>
+  <si>
+    <t>du côté (de)</t>
+  </si>
+  <si>
+    <t>dü ko.te. d@</t>
+  </si>
+  <si>
+    <t>po boku čeho</t>
+  </si>
+  <si>
+    <t>vedle (čeho)</t>
+  </si>
+  <si>
+    <t>à l'écart (de)</t>
+  </si>
+  <si>
+    <t>a le.ka:r d@</t>
+  </si>
+  <si>
+    <t>stranou (čeho)</t>
+  </si>
+  <si>
+    <t>dans les environs (de)</t>
+  </si>
+  <si>
+    <t>da~ le.za~viro~ d@</t>
+  </si>
+  <si>
+    <t>v okolí (čeho)</t>
+  </si>
+  <si>
+    <t>loin (de)</t>
+  </si>
+  <si>
+    <t>lu^e~ d@</t>
+  </si>
+  <si>
+    <t>daleko (od čeho)</t>
+  </si>
+  <si>
+    <t>au loin</t>
+  </si>
+  <si>
+    <t>o. lu^e~</t>
+  </si>
+  <si>
+    <t>v dálce, daleko</t>
+  </si>
+  <si>
+    <t>un peu plus loin</t>
+  </si>
+  <si>
+    <t>ö~ pö plü lu^e~</t>
+  </si>
+  <si>
+    <t>trochu dál</t>
+  </si>
+  <si>
+    <t>à mi-chemin</t>
+  </si>
+  <si>
+    <t>a miš@me~</t>
+  </si>
+  <si>
+    <t>v půli cesty, na půl cesty</t>
+  </si>
+  <si>
+    <t>à peu de distance de</t>
+  </si>
+  <si>
+    <t>a pö d@ dista~:s d@</t>
+  </si>
+  <si>
+    <t>na vzdálenost o málo kratší než</t>
+  </si>
+  <si>
+    <t>près (de)</t>
+  </si>
+  <si>
+    <t>pre d@</t>
+  </si>
+  <si>
+    <t>blízko (čeho)</t>
+  </si>
+  <si>
+    <t>tout près</t>
+  </si>
+  <si>
+    <t>tu pre</t>
+  </si>
+  <si>
+    <t>à proximité de</t>
+  </si>
+  <si>
+    <t>a proksimite. d@</t>
+  </si>
+  <si>
+    <t>v blízkosti čeho</t>
+  </si>
+  <si>
+    <t>dö~ bu a lo.tr</t>
+  </si>
+  <si>
+    <t>z jednoho konce na druhý</t>
+  </si>
+  <si>
+    <t>en chemin</t>
+  </si>
+  <si>
+    <t>a~ š@me~</t>
+  </si>
+  <si>
+    <t>na cestě, po cestě, cestou, mezitím</t>
+  </si>
+  <si>
+    <t>en direction de</t>
+  </si>
+  <si>
+    <t>a~ direksjo~ d@</t>
+  </si>
+  <si>
+    <t>směrem na co, směrem k čemu, ve směru čeho</t>
+  </si>
+  <si>
+    <t>dans la direction de</t>
+  </si>
+  <si>
+    <t>da~ la direksjo~ d@</t>
+  </si>
+  <si>
+    <t>směrem na co</t>
+  </si>
+  <si>
+    <t>tout droit</t>
+  </si>
+  <si>
+    <t>tu dru^a</t>
+  </si>
+  <si>
+    <t>přímo, pořád rovně</t>
+  </si>
+  <si>
+    <t>jusqu'à</t>
+  </si>
+  <si>
+    <t>žüska</t>
+  </si>
+  <si>
+    <t>až k (čemu)</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>přes</t>
+  </si>
+  <si>
+    <t>par la</t>
+  </si>
+  <si>
+    <t>à travers</t>
+  </si>
+  <si>
+    <t>a trave:r</t>
+  </si>
+  <si>
+    <t>napříč, přes co</t>
+  </si>
+  <si>
+    <t>sur la route de</t>
+  </si>
+  <si>
+    <t>sür la rut d@</t>
+  </si>
+  <si>
+    <t>na cestě k čemu</t>
+  </si>
+  <si>
+    <t>vers</t>
+  </si>
+  <si>
+    <t>ve:r</t>
+  </si>
+  <si>
+    <t>směrem k (čemu)</t>
   </si>
 </sst>
 </file>
@@ -2359,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2776,4 +3006,436 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "aux alentours", "grammar": "adv", "pronunciation": "o.zala~tu:r", "meaning": "v okolí" },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C8" t="s">
+        <v>298</v>
+      </c>
+      <c r="D8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D9" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>303</v>
+      </c>
+      <c r="C10" t="s">
+        <v>304</v>
+      </c>
+      <c r="D10" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>306</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
+        <v>307</v>
+      </c>
+      <c r="D11" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>309</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D12" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" t="s">
+        <v>313</v>
+      </c>
+      <c r="D13" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>315</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>318</v>
+      </c>
+      <c r="C15" t="s">
+        <v>319</v>
+      </c>
+      <c r="D15" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" t="s">
+        <v>322</v>
+      </c>
+      <c r="D16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>324</v>
+      </c>
+      <c r="D17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="55.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "d'un bout à l'autre", "grammar": "", "pronunciation": "dö~ bu a lo.tr", "meaning": "z jednoho konce na druhý" },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>343</v>
+      </c>
+      <c r="D8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" t="s">
+        <v>345</v>
+      </c>
+      <c r="D9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>346</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>347</v>
+      </c>
+      <c r="D10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>349</v>
+      </c>
+      <c r="C11" t="s">
+        <v>350</v>
+      </c>
+      <c r="D11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>352</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>353</v>
+      </c>
+      <c r="D12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CHANGE Miilon - Finish the vocabulary on the page 59 of EDITO.
</commit_message>
<xml_diff>
--- a/MiilonData/05_EditoB2_unite4_p59_Le_lieu.xlsx
+++ b/MiilonData/05_EditoB2_unite4_p59_Le_lieu.xlsx
@@ -2034,7 +2034,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,7 +2177,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F2" sqref="F2:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2634,6 +2634,10 @@
       <c r="D3" t="s">
         <v>189</v>
       </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F49" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "à l'arrière (de)", "grammar": "", "pronunciation": "", "meaning": "na zádi (čeho)" },</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2642,6 +2646,10 @@
       <c r="D4" t="s">
         <v>191</v>
       </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en arrière", "grammar": "", "pronunciation": "", "meaning": "vzadu, pozadu" },</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2650,6 +2658,10 @@
       <c r="D5" t="s">
         <v>193</v>
       </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au-delà de", "grammar": "", "pronunciation": "", "meaning": "za čím, na druhé straně čeho" },</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2658,6 +2670,10 @@
       <c r="D6" t="s">
         <v>195</v>
       </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "autour (de)", "grammar": "", "pronunciation": "", "meaning": "kolem (čeho)" },</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2666,6 +2682,10 @@
       <c r="D7" t="s">
         <v>197</v>
       </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "autre part", "grammar": "", "pronunciation": "", "meaning": "jinde" },</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2674,6 +2694,10 @@
       <c r="D8" t="s">
         <v>199</v>
       </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à l'avant (de)", "grammar": "", "pronunciation": "", "meaning": "na přídi (čeho)" },</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2682,6 +2706,10 @@
       <c r="D9" t="s">
         <v>201</v>
       </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en bas (de)", "grammar": "", "pronunciation": "", "meaning": "dole, v dolní části (čeho)" },</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2690,6 +2718,10 @@
       <c r="D10" t="s">
         <v>203</v>
       </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au bord (de)", "grammar": "", "pronunciation": "", "meaning": "na kraji (čeho)" },</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2698,6 +2730,10 @@
       <c r="D11" t="s">
         <v>205</v>
       </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au bout (de)", "grammar": "", "pronunciation": "", "meaning": "na konci (čeho)" },</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2706,6 +2742,10 @@
       <c r="D12" t="s">
         <v>207</v>
       </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au centre (de)", "grammar": "", "pronunciation": "", "meaning": "uprostřed (čeho)" },</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2714,6 +2754,10 @@
       <c r="D13" t="s">
         <v>209</v>
       </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au coin (de)", "grammar": "", "pronunciation": "", "meaning": "na rohu (čeho)" },</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2722,6 +2766,10 @@
       <c r="D14" t="s">
         <v>211</v>
       </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "dans un coin", "grammar": "", "pronunciation": "", "meaning": "v rohu" },</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2730,6 +2778,10 @@
       <c r="D15" t="s">
         <v>213</v>
       </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "sur le côté (de)", "grammar": "", "pronunciation": "", "meaning": "po straně / podél (čeho)" },</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2738,269 +2790,405 @@
       <c r="D16" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "dedans", "grammar": "", "pronunciation": "", "meaning": "uvnitř" },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>216</v>
       </c>
       <c r="D17" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "dehors", "grammar": "", "pronunciation": "", "meaning": "venku" },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>220</v>
       </c>
       <c r="D18" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au dehors de", "grammar": "", "pronunciation": "", "meaning": "vně čeho" },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>218</v>
       </c>
       <c r="D19" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en dehors de", "grammar": "", "pronunciation": "", "meaning": "kromě / mimo čeho" },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>222</v>
       </c>
       <c r="D20" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "derrière", "grammar": "", "pronunciation": "", "meaning": "za, vzadu" },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>224</v>
       </c>
       <c r="D21" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "dessous", "grammar": "", "pronunciation": "", "meaning": "dole, dolů, vespod, spodní část, spodek" },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>227</v>
       </c>
       <c r="D22" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au-dessous (de)", "grammar": "", "pronunciation": "", "meaning": "pod (čím)" },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>229</v>
       </c>
       <c r="D23" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en dessous (de)", "grammar": "", "pronunciation": "", "meaning": "pod (čím), níže než (co)" },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>231</v>
       </c>
       <c r="D24" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "par-dessous", "grammar": "", "pronunciation": "", "meaning": "ještě, více, dále, přes, kromě" },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>142</v>
       </c>
       <c r="D25" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "dans", "grammar": "", "pronunciation": "", "meaning": "v, do" },</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>233</v>
       </c>
       <c r="D26" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "devant", "grammar": "", "pronunciation": "", "meaning": "před" },</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>235</v>
       </c>
       <c r="D27" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au devant de", "grammar": "", "pronunciation": "", "meaning": "naproti komu, vstříc komu" },</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>237</v>
       </c>
       <c r="D28" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à (la) droite (de)", "grammar": "", "pronunciation": "", "meaning": "napravo od, vpravo" },</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>239</v>
       </c>
       <c r="D29" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "sur votre droite", "grammar": "", "pronunciation": "", "meaning": "po vaší pravici" },</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>241</v>
       </c>
       <c r="D30" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "entre", "grammar": "", "pronunciation": "", "meaning": "mezi" },</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>243</v>
       </c>
       <c r="D31" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "face à", "grammar": "", "pronunciation": "", "meaning": "proti čemu, naproti čemu" },</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>245</v>
       </c>
       <c r="D32" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "face à face", "grammar": "", "pronunciation": "", "meaning": "tváří v tvář" },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>247</v>
       </c>
       <c r="D33" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en face (de)", "grammar": "", "pronunciation": "", "meaning": "naproti (čemu)" },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>249</v>
       </c>
       <c r="D34" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au fond (de)", "grammar": "", "pronunciation": "", "meaning": "na dně (čeho)" },</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>251</v>
       </c>
       <c r="D35" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à (la) gauche (de)", "grammar": "", "pronunciation": "", "meaning": "napravo do, vpravo" },</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>253</v>
       </c>
       <c r="D36" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "sur votre gauche", "grammar": "", "pronunciation": "", "meaning": " po vaší levici" },</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>255</v>
       </c>
       <c r="D37" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en haut (de)", "grammar": "", "pronunciation": "", "meaning": "nahoře, nahoře na čem" },</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>257</v>
       </c>
       <c r="D38" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "de haut", "grammar": "", "pronunciation": "", "meaning": "seshora" },</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>259</v>
       </c>
       <c r="D39" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "hors de", "grammar": "", "pronunciation": "", "meaning": "mimo co" },</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>261</v>
       </c>
       <c r="D40" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "de là", "grammar": "", "pronunciation": "", "meaning": "odtud" },</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>263</v>
       </c>
       <c r="D41" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "par là", "grammar": "", "pronunciation": "", "meaning": "tudy" },</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>265</v>
       </c>
       <c r="D42" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au milieu (de)", "grammar": "", "pronunciation": "", "meaning": "uprostřed (čeho)" },</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>266</v>
       </c>
       <c r="D43" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au pied de", "grammar": "", "pronunciation": "", "meaning": "na úpatí čeho" },</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>268</v>
       </c>
       <c r="D44" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au sein de", "grammar": "", "pronunciation": "", "meaning": "uvnitř čeho, uprostřed čeho, v čem" },</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>270</v>
       </c>
       <c r="D45" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au seuil de", "grammar": "", "pronunciation": "", "meaning": "na prahu čeho, na počátku čeho" },</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>272</v>
       </c>
       <c r="D46" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "sous", "grammar": "", "pronunciation": "", "meaning": "pod" },</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>273</v>
       </c>
       <c r="D47" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "sur", "grammar": "", "pronunciation": "", "meaning": "nad, na" },</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>275</v>
       </c>
       <c r="D48" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à la tête de", "grammar": "", "pronunciation": "", "meaning": "v čele čeho" },</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>277</v>
       </c>
       <c r="D49" t="s">
         <v>278</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en tête (de)", "grammar": "", "pronunciation": "", "meaning": "v čele, na počátku, v záhlaví čeho" },</v>
       </c>
     </row>
   </sheetData>
@@ -3013,7 +3201,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F2" sqref="F2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3069,6 +3257,10 @@
       <c r="D3" t="s">
         <v>284</v>
       </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F17" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "contre", "grammar": "prép", "pronunciation": "ko~:tr", "meaning": "proti, naproti" },</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3083,6 +3275,10 @@
       <c r="D4" t="s">
         <v>287</v>
       </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "tout contre", "grammar": "adv", "pronunciation": "tu ko~:tr", "meaning": "zcela blízko" },</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -3094,6 +3290,10 @@
       <c r="D5" t="s">
         <v>290</v>
       </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à côté (de)", "grammar": "", "pronunciation": "a ko.te. d@", "meaning": "vedle (čeho), mimo" },</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3108,6 +3308,10 @@
       <c r="D6" t="s">
         <v>295</v>
       </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au côté de", "grammar": "prép", "pronunciation": "o. ko.te. d@", "meaning": "po boku čeho" },</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3119,6 +3323,10 @@
       <c r="D7" t="s">
         <v>296</v>
       </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "du côté (de)", "grammar": "", "pronunciation": "dü ko.te. d@", "meaning": "vedle (čeho)" },</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3130,6 +3338,10 @@
       <c r="D8" t="s">
         <v>299</v>
       </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à l'écart (de)", "grammar": "", "pronunciation": "a le.ka:r d@", "meaning": "stranou (čeho)" },</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -3141,6 +3353,10 @@
       <c r="D9" t="s">
         <v>302</v>
       </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "dans les environs (de)", "grammar": "", "pronunciation": "da~ le.za~viro~ d@", "meaning": "v okolí (čeho)" },</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3152,6 +3368,10 @@
       <c r="D10" t="s">
         <v>305</v>
       </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "loin (de)", "grammar": "", "pronunciation": "lu^e~ d@", "meaning": "daleko (od čeho)" },</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -3166,6 +3386,10 @@
       <c r="D11" t="s">
         <v>308</v>
       </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "au loin", "grammar": "adv", "pronunciation": "o. lu^e~", "meaning": "v dálce, daleko" },</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -3180,6 +3404,10 @@
       <c r="D12" t="s">
         <v>311</v>
       </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "un peu plus loin", "grammar": "adv", "pronunciation": "ö~ pö plü lu^e~", "meaning": "trochu dál" },</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3194,6 +3422,10 @@
       <c r="D13" t="s">
         <v>314</v>
       </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à mi-chemin", "grammar": "adv", "pronunciation": "a miš@me~", "meaning": "v půli cesty, na půl cesty" },</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3208,6 +3440,10 @@
       <c r="D14" t="s">
         <v>317</v>
       </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à peu de distance de", "grammar": "prép", "pronunciation": "a pö d@ dista~:s d@", "meaning": "na vzdálenost o málo kratší než" },</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3219,6 +3455,10 @@
       <c r="D15" t="s">
         <v>320</v>
       </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "près (de)", "grammar": "", "pronunciation": "pre d@", "meaning": "blízko (čeho)" },</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -3233,8 +3473,12 @@
       <c r="D16" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "tout près", "grammar": "adv", "pronunciation": "tu pre", "meaning": "zcela blízko" },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>323</v>
       </c>
@@ -3246,6 +3490,10 @@
       </c>
       <c r="D17" t="s">
         <v>325</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à proximité de", "grammar": "prép", "pronunciation": "a proksimite. d@", "meaning": "v blízkosti čeho" },</v>
       </c>
     </row>
   </sheetData>
@@ -3258,7 +3506,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F2" sqref="F2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3311,6 +3559,10 @@
       <c r="D3" t="s">
         <v>330</v>
       </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F12" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "en chemin", "grammar": "adv", "pronunciation": "a~ š@me~", "meaning": "na cestě, po cestě, cestou, mezitím" },</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3325,6 +3577,10 @@
       <c r="D4" t="s">
         <v>333</v>
       </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en direction de", "grammar": "prép", "pronunciation": "a~ direksjo~ d@", "meaning": "směrem na co, směrem k čemu, ve směru čeho" },</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -3339,6 +3595,10 @@
       <c r="D5" t="s">
         <v>336</v>
       </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "dans la direction de", "grammar": "prép", "pronunciation": "da~ la direksjo~ d@", "meaning": "směrem na co" },</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3353,6 +3613,10 @@
       <c r="D6" t="s">
         <v>339</v>
       </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "tout droit", "grammar": "adv", "pronunciation": "tu dru^a", "meaning": "přímo, pořád rovně" },</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3367,6 +3631,10 @@
       <c r="D7" t="s">
         <v>342</v>
       </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "jusqu'à", "grammar": "prép", "pronunciation": "žüska", "meaning": "až k (čemu)" },</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3381,6 +3649,10 @@
       <c r="D8" t="s">
         <v>344</v>
       </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "par", "grammar": "prép", "pronunciation": "par", "meaning": "přes" },</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -3395,6 +3667,10 @@
       <c r="D9" t="s">
         <v>264</v>
       </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "par là", "grammar": "adv", "pronunciation": "par la", "meaning": "tudy" },</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3409,6 +3685,10 @@
       <c r="D10" t="s">
         <v>348</v>
       </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à travers", "grammar": "prép", "pronunciation": "a trave:r", "meaning": "napříč, přes co" },</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -3420,6 +3700,10 @@
       <c r="D11" t="s">
         <v>351</v>
       </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "sur la route de", "grammar": "", "pronunciation": "sür la rut d@", "meaning": "na cestě k čemu" },</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -3433,6 +3717,10 @@
       </c>
       <c r="D12" t="s">
         <v>354</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "vers", "grammar": "prép", "pronunciation": "ve:r", "meaning": "směrem k (čemu)" },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>